<commit_message>
day 8 assigments updated
</commit_message>
<xml_diff>
--- a/day8/assignment/program1.xlsx
+++ b/day8/assignment/program1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pytohn_learning\Quest_python\day8\assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBE8D53F-E9A5-46EF-86E9-381DCE1F3469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB7A865-589A-4453-9646-ED2F39928EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{624FFF07-E32B-4795-AEDB-7625622E54E0}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{624FFF07-E32B-4795-AEDB-7625622E54E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
   <si>
     <t xml:space="preserve">use cases </t>
   </si>
@@ -90,13 +90,34 @@
     <t>&lt;35</t>
   </si>
   <si>
-    <t xml:space="preserve">no opening </t>
-  </si>
-  <si>
     <t>&lt;90</t>
   </si>
   <si>
     <t>&lt;95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">your marks do not qualify </t>
+  </si>
+  <si>
+    <t xml:space="preserve">marks do not qualify </t>
+  </si>
+  <si>
+    <t xml:space="preserve">marks do not qualify  </t>
+  </si>
+  <si>
+    <t>preference do not match</t>
+  </si>
+  <si>
+    <t>mech</t>
+  </si>
+  <si>
+    <t>actual op</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -448,20 +469,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0271103-19C0-4A8C-BAC5-A88E254B97B4}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -474,8 +495,14 @@
       <c r="H2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -486,7 +513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -505,8 +532,14 @@
       <c r="H4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -525,8 +558,14 @@
       <c r="H5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -545,8 +584,14 @@
       <c r="H6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -560,15 +605,21 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -583,15 +634,21 @@
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -603,7 +660,91 @@
         <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>